<commit_message>
code refactor and Excel methods added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/AccountCallback.xlsx
+++ b/src/test/resources/testData/AccountCallback.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fkara\Desktop\workspace\EfecturaTestAutomation\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fkara\Desktop\workspace1\EfecturaTestAutomation\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBF8822-CC48-4993-8AEB-BA392D46A784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A7DB29-97C5-4970-B332-F1A4E7556352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3936" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>AccountNumber</t>
   </si>
@@ -63,12 +63,6 @@
     <t>5070545544</t>
   </si>
   <si>
-    <t>-120</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>20-02-2025</t>
   </si>
   <si>
@@ -76,9 +70,6 @@
   </si>
   <si>
     <t>53550</t>
-  </si>
-  <si>
-    <t>BJLSLAOV5X</t>
   </si>
   <si>
     <t>3XFQY4OGXA</t>
@@ -94,7 +85,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -507,20 +497,20 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="30.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="23.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="25.5546875" collapsed="true"/>
-    <col min="4" max="4" style="2" width="9.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="21.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="2" width="18.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="15.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="2" width="12.88671875" collapsed="true"/>
-    <col min="9" max="16384" style="2" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="30.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.5546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.109375" style="2" collapsed="1"/>
+    <col min="5" max="5" width="21.5546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.5546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.88671875" style="2" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.109375" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.8" x14ac:dyDescent="0.3">
@@ -557,22 +547,22 @@
         <v>10</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>11</v>

</xml_diff>